<commit_message>
Adding Remaing RBL documets
</commit_message>
<xml_diff>
--- a/Documents/RBL/RBL API List.xlsx
+++ b/Documents/RBL/RBL API List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\UKMF_Laravel\Documents\RBL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="275">
   <si>
     <t>Aadhaar Pay API Product</t>
   </si>
@@ -726,13 +726,179 @@
   </si>
   <si>
     <t>The office locator is a mapping solution for searching locations or RBL bank branch and ATMs with their addresses. Benefits: a) Find us anywhere in India, b) Compare RBL Bank Rates with competition Banks.</t>
+  </si>
+  <si>
+    <t>Remittance Account Inquiry API</t>
+  </si>
+  <si>
+    <t>This API specifically catering to regulatory guidelines for RDA product</t>
+  </si>
+  <si>
+    <t>RuleEngine-PowerCurvePL API</t>
+  </si>
+  <si>
+    <t>PowerCurve PL module to be integrated with channel partners. Powercurve application decides the validity of PL basis Customer demographics, Cibil output and multiple other variables. There is rule engine in the application which calculates whether a Loan should be given to the customer or not.</t>
+  </si>
+  <si>
+    <t>CCUBP_SIDebit &amp; Notification API</t>
+  </si>
+  <si>
+    <t>It will be used to debit amount by using ONUS on basis of input parameters</t>
+  </si>
+  <si>
+    <t>Single Payment API for Foreign Remittance RDA API</t>
+  </si>
+  <si>
+    <t>This API will facilitate the client to initiate payment under RDA arrangement for Foreign Remittances.</t>
+  </si>
+  <si>
+    <t>OAuth Provider API for Single Payment</t>
+  </si>
+  <si>
+    <t>Single Payment API with provider</t>
+  </si>
+  <si>
+    <t>RBL Single Payment API (OAuth)</t>
+  </si>
+  <si>
+    <t>/this API is used to carry out a single payment</t>
+  </si>
+  <si>
+    <t>Single Payment with BeneID</t>
+  </si>
+  <si>
+    <t>Statement with Remitter Details API</t>
+  </si>
+  <si>
+    <t>AccountBalanceTemp</t>
+  </si>
+  <si>
+    <t>This is account bal</t>
+  </si>
+  <si>
+    <t>Term Loan account opening</t>
+  </si>
+  <si>
+    <t>This service is being used for Term Loan account opening through ESB layer for Personal Loan type loan with having only EI repayment under SWADHAR scheme and ARTOO is the technical partner.</t>
+  </si>
+  <si>
+    <t>Collection Test API</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>test-oauth</t>
+  </si>
+  <si>
+    <t>test-oauth-api</t>
+  </si>
+  <si>
+    <t>Trade Finance Inquiry API</t>
+  </si>
+  <si>
+    <t>Trade Pro API</t>
+  </si>
+  <si>
+    <t>UPI Collections API</t>
+  </si>
+  <si>
+    <t>The UPI platform aims at facilitating payments and provides 24x7 services for payment processing. The payments are processed quickly and seamlessly without exposing the account details. All banks can avail of the UPI services and be a part of next generation payment network as Payment Service Player (PSP). For this, banks need to integrate with the services exposed by UPI.Through RBL a registered user can raise request for money from another registered user. Funds will be transferred when the user authorizes the collection.</t>
+  </si>
+  <si>
+    <t>UPI Payment API</t>
+  </si>
+  <si>
+    <t>Payment API will be used by the Partner for the requirement of Paying/Disbursing the money to the other customer via VPA mode.</t>
+  </si>
+  <si>
+    <t>URN Validation</t>
+  </si>
+  <si>
+    <t>API to be developed which basically validate URN NO which will be passed and gives response with the customer details.</t>
+  </si>
+  <si>
+    <t>Collection Recon API</t>
+  </si>
+  <si>
+    <t>Virtual Account API</t>
+  </si>
+  <si>
+    <t>Virtual account API facilitates to create a virtual account for the request sent. And, you can modernize the way of managing multiple accounts/clients, preferably suitable for high transaction volumes, flexible to activate/de-activate or modify the virtual account and allow you a secure and seamless integration with RBL Bank’s Payment services. It provides for 1)Virtual Account Request: Create a virtual account. The client can create multiple virtual accounts under one customer id or account number. The virtual accounts are maintained in following format i.e. VA&lt;5 alphanumeric code&gt;&lt;20 digit allocated to sender details&gt; 2)Virtual Account Inquiry Response: The client can retrieve virtual account number, client id and name of the virtual account from the database.</t>
+  </si>
+  <si>
+    <t>Questions</t>
+  </si>
+  <si>
+    <t>Does, This API all banks details like Yes Bank,SBI,PNB etc ? Or It's just retrieve details of account create under RBL system ?</t>
+  </si>
+  <si>
+    <t>1. Did we have JSON Support ?
+2. Payment Mode type ?</t>
+  </si>
+  <si>
+    <t>1. Account need to Assocated with RBL ?
+If Yes than does this work on virtual Accounts.
+Also card exp date,CVV1,CVV2,Activation and Auth token on those virtual card will work for payment viz NFC ?</t>
+  </si>
+  <si>
+    <t>Can you share detail process ? How system work.</t>
+  </si>
+  <si>
+    <t>Color Code meaning</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t xml:space="preserve"> 1. Yellow - required API for Wallet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t>2. Light Blue API - which provide extra features to wallet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t>3. Light Orange - API which needfull for other projects.</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Did we have JSON Support ?
+2. UPI Payment refund/Failer handling ?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -744,16 +910,82 @@
       <sz val="11"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -761,20 +993,71 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1056,1774 +1339,2239 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D163"/>
+  <dimension ref="A1:G163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C109" sqref="C109"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A86" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="122" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.5703125" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="1.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="11" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="36">
+      <c r="B1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="11" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="F1" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1">
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="242.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="135" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="2" customFormat="1" ht="57">
+      <c r="A4" s="6"/>
+      <c r="B4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="405" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" s="2" customFormat="1" ht="114">
+      <c r="A5" s="7"/>
+      <c r="B5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="165" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="F5" s="12" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="2" customFormat="1" ht="57">
+      <c r="A6" s="4"/>
+      <c r="B6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="3" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" s="2" customFormat="1" ht="57">
+      <c r="A7" s="4"/>
+      <c r="B7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="285" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="E7" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" s="2" customFormat="1" ht="85.5">
+      <c r="A8" s="4"/>
+      <c r="B8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="3" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" s="2" customFormat="1" ht="57">
+      <c r="A9" s="4"/>
+      <c r="B9" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="E9" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" s="2" customFormat="1" ht="42.75">
+      <c r="A10" s="4"/>
+      <c r="B10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="180" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="E10" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" s="2" customFormat="1" ht="57">
+      <c r="A11" s="4"/>
+      <c r="B11" s="3">
         <v>9</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="3" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" s="2" customFormat="1" ht="171">
+      <c r="A12" s="7"/>
+      <c r="B12" s="3">
         <v>10</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="3" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="F12" s="12" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="2" customFormat="1" ht="114">
+      <c r="A13" s="4"/>
+      <c r="B13" s="3">
         <v>11</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="3" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" s="2" customFormat="1" ht="409.5">
+      <c r="A14" s="6"/>
+      <c r="B14" s="3">
         <v>12</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="3" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="F14" s="12" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="2" customFormat="1" ht="42.75">
+      <c r="A15" s="4"/>
+      <c r="B15" s="3">
         <v>13</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="180" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="E15" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" s="2" customFormat="1" ht="57">
+      <c r="A16" s="13"/>
+      <c r="B16" s="3">
         <v>14</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="3" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" s="2" customFormat="1" ht="57">
+      <c r="A17" s="4"/>
+      <c r="B17" s="3">
         <v>15</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="E17" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" s="2" customFormat="1" ht="142.5">
+      <c r="A18" s="4"/>
+      <c r="B18" s="3">
         <v>16</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="3" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" s="2" customFormat="1" ht="42.75">
+      <c r="A19" s="4"/>
+      <c r="B19" s="3">
         <v>17</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+      <c r="E19" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" s="2" customFormat="1" ht="42.75">
+      <c r="A20" s="4"/>
+      <c r="B20" s="3">
         <v>18</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="3" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" s="2" customFormat="1" ht="28.5">
+      <c r="A21" s="4"/>
+      <c r="B21" s="3">
         <v>19</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+      <c r="E21" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" s="2" customFormat="1" ht="28.5">
+      <c r="A22" s="4"/>
+      <c r="B22" s="15">
         <v>20</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="2" t="s">
+      <c r="E22" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" s="2" customFormat="1">
+      <c r="A23" s="13"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="2" t="s">
+      <c r="E23" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" s="2" customFormat="1">
+      <c r="A24" s="13"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+      <c r="E24" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" s="2" customFormat="1" ht="28.5">
+      <c r="A25" s="4"/>
+      <c r="B25" s="3">
         <v>21</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+      <c r="E25" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" s="2" customFormat="1" ht="57">
+      <c r="A26" s="14"/>
+      <c r="B26" s="3">
         <v>22</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+      <c r="E26" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" s="2" customFormat="1" ht="42.75">
+      <c r="A27" s="4"/>
+      <c r="B27" s="3">
         <v>23</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+      <c r="E27" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" s="2" customFormat="1" ht="114">
+      <c r="A28" s="4"/>
+      <c r="B28" s="3">
         <v>24</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="3" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:6" s="2" customFormat="1" ht="57">
+      <c r="A29" s="4"/>
+      <c r="B29" s="3">
         <v>25</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="3" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:6" s="2" customFormat="1" ht="57">
+      <c r="A30" s="4"/>
+      <c r="B30" s="3">
         <v>26</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" s="2" customFormat="1" ht="242.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="3">
         <v>27</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="3" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" s="2" customFormat="1" ht="42.75">
+      <c r="A32" s="4"/>
+      <c r="B32" s="3">
         <v>28</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+      <c r="E32" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="1:6" s="2" customFormat="1" ht="57">
+      <c r="A33" s="4"/>
+      <c r="B33" s="3">
         <v>29</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="E33" s="3" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="1:6" s="2" customFormat="1" ht="71.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="3">
         <v>30</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+      <c r="E34" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="1:6" s="2" customFormat="1" ht="42.75">
+      <c r="A35" s="4"/>
+      <c r="B35" s="3">
         <v>31</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
+      <c r="E35" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="1:6" s="2" customFormat="1" ht="42.75">
+      <c r="A36" s="4"/>
+      <c r="B36" s="3">
         <v>32</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="E36" s="3" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" spans="1:6" s="2" customFormat="1" ht="28.5">
+      <c r="A37" s="4"/>
+      <c r="B37" s="15">
         <v>33</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="C37" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="2" t="s">
+      <c r="E37" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="1:6" s="2" customFormat="1" ht="42.75">
+      <c r="A38" s="4"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="E38" s="3" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="2" t="s">
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="1:6" s="2" customFormat="1">
+      <c r="A39" s="4"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="2" t="s">
+      <c r="E39" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40" spans="1:6" s="2" customFormat="1">
+      <c r="A40" s="4"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="2" t="s">
+      <c r="E40" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41" spans="1:6" s="2" customFormat="1">
+      <c r="A41" s="4"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="2" t="s">
+      <c r="E41" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="1:6" s="2" customFormat="1">
+      <c r="A42" s="4"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
+      <c r="E42" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F42" s="3"/>
+    </row>
+    <row r="43" spans="1:6" s="2" customFormat="1" ht="57">
+      <c r="A43" s="4"/>
+      <c r="B43" s="3">
         <v>34</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="C43" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="D43" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
+      <c r="E43" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F43" s="3"/>
+    </row>
+    <row r="44" spans="1:6" s="2" customFormat="1" ht="57">
+      <c r="A44" s="4"/>
+      <c r="B44" s="3">
         <v>35</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="C44" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="E44" s="3" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
+      <c r="F44" s="3"/>
+    </row>
+    <row r="45" spans="1:6" s="2" customFormat="1" ht="128.25">
+      <c r="A45" s="6"/>
+      <c r="B45" s="3">
         <v>36</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="C45" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="D45" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="E45" s="3" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="3">
+      <c r="F45" s="3"/>
+    </row>
+    <row r="46" spans="1:6" s="2" customFormat="1" ht="42.75">
+      <c r="A46" s="4"/>
+      <c r="B46" s="15">
         <v>37</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="C46" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="D46" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="E46" s="3" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="2" t="s">
+      <c r="F46" s="3"/>
+    </row>
+    <row r="47" spans="1:6" s="2" customFormat="1" ht="57">
+      <c r="A47" s="4"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="E47" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
+      <c r="F47" s="3"/>
+    </row>
+    <row r="48" spans="1:6" s="2" customFormat="1" ht="57">
+      <c r="A48" s="4"/>
+      <c r="B48" s="3">
         <v>38</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="C48" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="D48" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
+      <c r="E48" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F48" s="3"/>
+    </row>
+    <row r="49" spans="1:6" s="2" customFormat="1" ht="171">
+      <c r="A49" s="4"/>
+      <c r="B49" s="3">
         <v>39</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="C49" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="D49" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="E49" s="3" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="2">
+      <c r="F49" s="3"/>
+    </row>
+    <row r="50" spans="1:6" s="2" customFormat="1" ht="42.75">
+      <c r="A50" s="4"/>
+      <c r="B50" s="3">
         <v>40</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="C50" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
+      <c r="D50" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F50" s="3"/>
+    </row>
+    <row r="51" spans="1:6" s="2" customFormat="1" ht="171">
+      <c r="A51" s="4"/>
+      <c r="B51" s="3">
         <v>41</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="C51" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="D51" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="E51" s="3" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="2">
+      <c r="F51" s="3"/>
+    </row>
+    <row r="52" spans="1:6" s="2" customFormat="1" ht="71.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="3">
         <v>42</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="C52" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="D52" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="E52" s="3" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="2">
+      <c r="F52" s="3"/>
+    </row>
+    <row r="53" spans="1:6" s="2" customFormat="1" ht="28.5">
+      <c r="A53" s="4"/>
+      <c r="B53" s="3">
         <v>43</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="C53" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="2">
+      <c r="D53" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F53" s="3"/>
+    </row>
+    <row r="54" spans="1:6" s="2" customFormat="1" ht="42.75">
+      <c r="A54" s="4"/>
+      <c r="B54" s="3">
         <v>44</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="C54" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="2">
+      <c r="D54" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F54" s="3"/>
+    </row>
+    <row r="55" spans="1:6" s="2" customFormat="1" ht="42.75">
+      <c r="A55" s="7"/>
+      <c r="B55" s="3">
         <v>45</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="C55" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="2">
+      <c r="D55" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F55" s="3"/>
+    </row>
+    <row r="56" spans="1:6" s="2" customFormat="1" ht="57">
+      <c r="A56" s="4"/>
+      <c r="B56" s="3">
         <v>46</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="C56" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="D56" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="D56" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="2">
+      <c r="E56" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F56" s="3"/>
+    </row>
+    <row r="57" spans="1:6" s="2" customFormat="1" ht="28.5">
+      <c r="A57" s="4"/>
+      <c r="B57" s="3">
         <v>47</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="C57" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="D57" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D57" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="2">
+      <c r="E57" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F57" s="3"/>
+    </row>
+    <row r="58" spans="1:6" s="2" customFormat="1" ht="42.75">
+      <c r="A58" s="4"/>
+      <c r="B58" s="3">
         <v>48</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="C58" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="D58" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="D58" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="2">
+      <c r="E58" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F58" s="3"/>
+    </row>
+    <row r="59" spans="1:6" s="2" customFormat="1" ht="42.75">
+      <c r="A59" s="4"/>
+      <c r="B59" s="3">
         <v>49</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="C59" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="D59" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="E59" s="3" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="2">
+      <c r="F59" s="3"/>
+    </row>
+    <row r="60" spans="1:6" s="2" customFormat="1" ht="42.75">
+      <c r="A60" s="4"/>
+      <c r="B60" s="3">
         <v>50</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="C60" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="D60" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="E60" s="3" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="2">
+      <c r="F60" s="3"/>
+    </row>
+    <row r="61" spans="1:6" s="2" customFormat="1" ht="57">
+      <c r="A61" s="4"/>
+      <c r="B61" s="3">
         <v>51</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="C61" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="D61" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D61" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="2">
+      <c r="E61" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F61" s="3"/>
+    </row>
+    <row r="62" spans="1:6" s="2" customFormat="1" ht="42.75">
+      <c r="A62" s="4"/>
+      <c r="B62" s="3">
         <v>52</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="C62" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="D62" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="2">
+      <c r="E62" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F62" s="3"/>
+    </row>
+    <row r="63" spans="1:6" s="2" customFormat="1" ht="42.75">
+      <c r="A63" s="4"/>
+      <c r="B63" s="3">
         <v>53</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="C63" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="D63" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="D63" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="2">
+      <c r="E63" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F63" s="3"/>
+    </row>
+    <row r="64" spans="1:6" s="2" customFormat="1" ht="42.75">
+      <c r="A64" s="4"/>
+      <c r="B64" s="3">
         <v>54</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="C64" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="D64" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="2">
+      <c r="E64" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F64" s="3"/>
+    </row>
+    <row r="65" spans="1:6" s="2" customFormat="1" ht="28.5">
+      <c r="A65" s="4"/>
+      <c r="B65" s="3">
         <v>55</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="C65" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C65" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="2">
+      <c r="D65" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F65" s="3"/>
+    </row>
+    <row r="66" spans="1:6" s="2" customFormat="1" ht="114">
+      <c r="A66" s="4"/>
+      <c r="B66" s="3">
         <v>56</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="C66" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="D66" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="E66" s="3" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="2">
+      <c r="F66" s="3"/>
+    </row>
+    <row r="67" spans="1:6" s="2" customFormat="1" ht="42.75">
+      <c r="A67" s="4"/>
+      <c r="B67" s="3">
         <v>57</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="C67" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="D67" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="E67" s="3" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="2">
+      <c r="F67" s="3"/>
+    </row>
+    <row r="68" spans="1:6" s="2" customFormat="1" ht="28.5">
+      <c r="A68" s="4"/>
+      <c r="B68" s="3">
         <v>58</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="C68" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C68" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="2">
+      <c r="D68" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F68" s="3"/>
+    </row>
+    <row r="69" spans="1:6" s="2" customFormat="1" ht="28.5">
+      <c r="A69" s="4"/>
+      <c r="B69" s="3">
         <v>59</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="C69" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="D69" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="D69" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="3">
+      <c r="E69" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F69" s="3"/>
+    </row>
+    <row r="70" spans="1:6" s="2" customFormat="1">
+      <c r="A70" s="4"/>
+      <c r="B70" s="15">
         <v>60</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="C70" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="D70" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D70" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="3"/>
-      <c r="B71" s="3"/>
-      <c r="C71" s="2" t="s">
+      <c r="E70" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F70" s="3"/>
+    </row>
+    <row r="71" spans="1:6" s="2" customFormat="1">
+      <c r="A71" s="4"/>
+      <c r="B71" s="15"/>
+      <c r="C71" s="15"/>
+      <c r="D71" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D71" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="3"/>
-      <c r="B72" s="3"/>
-      <c r="C72" s="2" t="s">
+      <c r="E71" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F71" s="3"/>
+    </row>
+    <row r="72" spans="1:6" s="2" customFormat="1">
+      <c r="A72" s="4"/>
+      <c r="B72" s="15"/>
+      <c r="C72" s="15"/>
+      <c r="D72" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D72" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="3"/>
-      <c r="B73" s="3"/>
-      <c r="C73" s="2" t="s">
+      <c r="E72" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F72" s="3"/>
+    </row>
+    <row r="73" spans="1:6" s="2" customFormat="1" ht="28.5">
+      <c r="A73" s="4"/>
+      <c r="B73" s="15"/>
+      <c r="C73" s="15"/>
+      <c r="D73" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="D73" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="2" t="s">
+      <c r="E73" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F73" s="3"/>
+    </row>
+    <row r="74" spans="1:6" s="2" customFormat="1" ht="128.25">
+      <c r="A74" s="4"/>
+      <c r="B74" s="15"/>
+      <c r="C74" s="15"/>
+      <c r="D74" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="E74" s="3" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="3"/>
-      <c r="B75" s="3"/>
-      <c r="C75" s="2" t="s">
+      <c r="F74" s="3"/>
+    </row>
+    <row r="75" spans="1:6" s="2" customFormat="1" ht="142.5">
+      <c r="A75" s="4"/>
+      <c r="B75" s="15"/>
+      <c r="C75" s="15"/>
+      <c r="D75" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="E75" s="3" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="3"/>
-      <c r="B76" s="3"/>
-      <c r="C76" s="2" t="s">
+      <c r="F75" s="3"/>
+    </row>
+    <row r="76" spans="1:6" s="2" customFormat="1">
+      <c r="A76" s="4"/>
+      <c r="B76" s="15"/>
+      <c r="C76" s="15"/>
+      <c r="D76" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="D76" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="3"/>
-      <c r="B77" s="3"/>
-      <c r="C77" s="2" t="s">
+      <c r="E76" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F76" s="3"/>
+    </row>
+    <row r="77" spans="1:6" s="2" customFormat="1" ht="28.5">
+      <c r="A77" s="4"/>
+      <c r="B77" s="15"/>
+      <c r="C77" s="15"/>
+      <c r="D77" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="3"/>
-      <c r="B78" s="3"/>
-      <c r="C78" s="2" t="s">
+      <c r="E77" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F77" s="3"/>
+    </row>
+    <row r="78" spans="1:6" s="2" customFormat="1">
+      <c r="A78" s="4"/>
+      <c r="B78" s="15"/>
+      <c r="C78" s="15"/>
+      <c r="D78" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D78" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="3"/>
-      <c r="B79" s="3"/>
-      <c r="C79" s="2" t="s">
+      <c r="E78" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F78" s="3"/>
+    </row>
+    <row r="79" spans="1:6" s="2" customFormat="1" ht="28.5">
+      <c r="A79" s="4"/>
+      <c r="B79" s="15"/>
+      <c r="C79" s="15"/>
+      <c r="D79" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="D79" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="2">
+      <c r="E79" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F79" s="3"/>
+    </row>
+    <row r="80" spans="1:6" s="2" customFormat="1" ht="71.25">
+      <c r="A80" s="7"/>
+      <c r="B80" s="3">
         <v>61</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="C80" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="D80" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="E80" s="3" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="2">
+      <c r="F80" s="3"/>
+    </row>
+    <row r="81" spans="1:6" s="2" customFormat="1" ht="28.5">
+      <c r="A81" s="4"/>
+      <c r="B81" s="3">
         <v>62</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="C81" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C81" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="2">
+      <c r="D81" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F81" s="3"/>
+    </row>
+    <row r="82" spans="1:6" s="2" customFormat="1" ht="57">
+      <c r="A82" s="4"/>
+      <c r="B82" s="3">
         <v>63</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="C82" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="D82" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="D82" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="2">
+      <c r="E82" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F82" s="3"/>
+    </row>
+    <row r="83" spans="1:6" s="2" customFormat="1" ht="28.5">
+      <c r="A83" s="4"/>
+      <c r="B83" s="3">
         <v>64</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="C83" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="D83" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="D83" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="2">
+      <c r="E83" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F83" s="3"/>
+    </row>
+    <row r="84" spans="1:6" s="2" customFormat="1" ht="42.75">
+      <c r="A84" s="4"/>
+      <c r="B84" s="3">
         <v>65</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="C84" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="D84" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="D84" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" s="2">
+      <c r="E84" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F84" s="3"/>
+    </row>
+    <row r="85" spans="1:6" s="2" customFormat="1" ht="114">
+      <c r="A85" s="4"/>
+      <c r="B85" s="3">
         <v>66</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="C85" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="D85" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="D85" s="1" t="s">
+      <c r="E85" s="3" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A86" s="2">
+      <c r="F85" s="3"/>
+    </row>
+    <row r="86" spans="1:6" s="2" customFormat="1" ht="313.5">
+      <c r="A86" s="7"/>
+      <c r="B86" s="3">
         <v>67</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="C86" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C86" s="2" t="s">
+      <c r="D86" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D86" s="1" t="s">
+      <c r="E86" s="3" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A87" s="2">
+      <c r="F86" s="3"/>
+    </row>
+    <row r="87" spans="1:6" s="2" customFormat="1" ht="342">
+      <c r="A87" s="6"/>
+      <c r="B87" s="3">
         <v>68</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="C87" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="D87" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="D87" s="1" t="s">
+      <c r="E87" s="3" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="2">
+      <c r="F87" s="12" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" s="2" customFormat="1" ht="42.75">
+      <c r="A88" s="4"/>
+      <c r="B88" s="3">
         <v>69</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="C88" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="D88" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="D88" s="1" t="s">
+      <c r="E88" s="3" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="2">
+      <c r="F88" s="3"/>
+    </row>
+    <row r="89" spans="1:6" s="2" customFormat="1" ht="42.75">
+      <c r="A89" s="4"/>
+      <c r="B89" s="3">
         <v>70</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="C89" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="D89" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="D89" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="2">
+      <c r="E89" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F89" s="3"/>
+    </row>
+    <row r="90" spans="1:6" s="2" customFormat="1" ht="42.75">
+      <c r="A90" s="7"/>
+      <c r="B90" s="3">
         <v>71</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="C90" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C90" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="2">
+      <c r="D90" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F90" s="3"/>
+    </row>
+    <row r="91" spans="1:6" s="2" customFormat="1" ht="28.5">
+      <c r="A91" s="4"/>
+      <c r="B91" s="3">
         <v>72</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="C91" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C91" s="2" t="s">
+      <c r="D91" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="D91" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="2">
+      <c r="E91" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F91" s="3"/>
+    </row>
+    <row r="92" spans="1:6" s="2" customFormat="1" ht="42.75">
+      <c r="A92" s="6"/>
+      <c r="B92" s="3">
         <v>73</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="C92" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="D92" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="D92" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A93" s="3">
+      <c r="E92" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F92" s="12" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" s="2" customFormat="1" ht="409.5">
+      <c r="A93" s="7"/>
+      <c r="B93" s="15">
         <v>74</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="C93" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="D93" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D93" s="1" t="s">
+      <c r="E93" s="3" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A94" s="3"/>
-      <c r="B94" s="3"/>
-      <c r="C94" s="2" t="s">
+      <c r="F93" s="3"/>
+    </row>
+    <row r="94" spans="1:6" s="2" customFormat="1" ht="171">
+      <c r="A94" s="4"/>
+      <c r="B94" s="15"/>
+      <c r="C94" s="15"/>
+      <c r="D94" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="D94" s="1" t="s">
+      <c r="E94" s="3" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="2">
+      <c r="F94" s="3"/>
+    </row>
+    <row r="95" spans="1:6" s="2" customFormat="1" ht="57">
+      <c r="A95" s="6"/>
+      <c r="B95" s="3">
         <v>75</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="C95" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C95" s="2" t="s">
+      <c r="D95" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="D95" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="2">
+      <c r="E95" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F95" s="3"/>
+    </row>
+    <row r="96" spans="1:6" s="2" customFormat="1" ht="57">
+      <c r="A96" s="4"/>
+      <c r="B96" s="3">
         <v>76</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="C96" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C96" s="2" t="s">
+      <c r="D96" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="D96" s="1" t="s">
+      <c r="E96" s="3" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="2">
+      <c r="F96" s="3"/>
+    </row>
+    <row r="97" spans="1:6" s="2" customFormat="1" ht="57">
+      <c r="A97" s="4"/>
+      <c r="B97" s="3">
         <v>77</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="C97" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="D97" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="D97" s="1" t="s">
+      <c r="E97" s="3" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="2">
+      <c r="F97" s="3"/>
+    </row>
+    <row r="98" spans="1:6" s="2" customFormat="1" ht="85.5">
+      <c r="A98" s="4"/>
+      <c r="B98" s="3">
         <v>78</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="C98" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C98" s="2" t="s">
+      <c r="D98" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="D98" s="1" t="s">
+      <c r="E98" s="3" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A99" s="2">
+      <c r="F98" s="3"/>
+    </row>
+    <row r="99" spans="1:6" s="2" customFormat="1" ht="99.75">
+      <c r="A99" s="6"/>
+      <c r="B99" s="3">
         <v>79</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="C99" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="D99" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D99" s="1" t="s">
+      <c r="E99" s="3" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="2">
+      <c r="F99" s="3"/>
+    </row>
+    <row r="100" spans="1:6" s="2" customFormat="1" ht="99.75">
+      <c r="A100" s="6"/>
+      <c r="B100" s="3">
         <v>80</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="C100" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="D100" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="D100" s="1" t="s">
+      <c r="E100" s="3" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="2">
+      <c r="F100" s="3"/>
+    </row>
+    <row r="101" spans="1:6" s="2" customFormat="1" ht="28.5">
+      <c r="A101" s="6"/>
+      <c r="B101" s="3">
         <v>81</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="C101" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="D101" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D101" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="2">
+      <c r="E101" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F101" s="3"/>
+    </row>
+    <row r="102" spans="1:6" s="2" customFormat="1" ht="71.25">
+      <c r="A102" s="6"/>
+      <c r="B102" s="3">
         <v>82</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="C102" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="D102" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="D102" s="1" t="s">
+      <c r="E102" s="3" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A103" s="2">
+      <c r="F102" s="3"/>
+    </row>
+    <row r="103" spans="1:6" s="2" customFormat="1" ht="85.5">
+      <c r="A103" s="6"/>
+      <c r="B103" s="3">
         <v>83</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="C103" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C103" s="2" t="s">
+      <c r="D103" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="D103" s="1" t="s">
+      <c r="E103" s="3" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A104" s="2">
+      <c r="F103" s="3"/>
+    </row>
+    <row r="104" spans="1:6" s="2" customFormat="1" ht="142.5">
+      <c r="A104" s="7"/>
+      <c r="B104" s="3">
         <v>84</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="C104" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C104" s="2" t="s">
+      <c r="D104" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="D104" s="1" t="s">
+      <c r="E104" s="3" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="3">
+      <c r="F104" s="3"/>
+    </row>
+    <row r="105" spans="1:6" s="2" customFormat="1" ht="114">
+      <c r="A105" s="6"/>
+      <c r="B105" s="15">
         <v>85</v>
       </c>
-      <c r="B105" s="3" t="s">
+      <c r="C105" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="C105" s="2" t="s">
+      <c r="D105" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="D105" s="1" t="s">
+      <c r="E105" s="3" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="3"/>
-      <c r="B106" s="3"/>
-      <c r="C106" s="2" t="s">
+      <c r="F105" s="3"/>
+    </row>
+    <row r="106" spans="1:6" s="2" customFormat="1" ht="156.75">
+      <c r="A106" s="6"/>
+      <c r="B106" s="15"/>
+      <c r="C106" s="15"/>
+      <c r="D106" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="D106" s="1" t="s">
+      <c r="E106" s="3" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="3"/>
-      <c r="B107" s="3"/>
-      <c r="C107" s="2" t="s">
+      <c r="F106" s="3"/>
+    </row>
+    <row r="107" spans="1:6" s="2" customFormat="1" ht="99.75">
+      <c r="A107" s="4"/>
+      <c r="B107" s="15"/>
+      <c r="C107" s="15"/>
+      <c r="D107" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="D107" s="1" t="s">
+      <c r="E107" s="3" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="3"/>
-      <c r="B108" s="3"/>
-      <c r="C108" s="2" t="s">
+      <c r="F107" s="3"/>
+    </row>
+    <row r="108" spans="1:6" s="2" customFormat="1" ht="128.25">
+      <c r="A108" s="4"/>
+      <c r="B108" s="15"/>
+      <c r="C108" s="15"/>
+      <c r="D108" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="D108" s="1" t="s">
+      <c r="E108" s="3" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="2">
+      <c r="F108" s="3"/>
+    </row>
+    <row r="109" spans="1:6" s="2" customFormat="1" ht="57">
+      <c r="A109" s="4"/>
+      <c r="B109" s="3">
         <v>86</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="C109" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D109" s="1"/>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="2">
+      <c r="D109" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="F109" s="3"/>
+    </row>
+    <row r="110" spans="1:6" s="2" customFormat="1" ht="185.25">
+      <c r="A110" s="4"/>
+      <c r="B110" s="3">
         <v>87</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="C110" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D110" s="1"/>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="2">
+      <c r="D110" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="F110" s="3"/>
+    </row>
+    <row r="111" spans="1:6" s="2" customFormat="1" ht="42.75">
+      <c r="A111" s="4"/>
+      <c r="B111" s="3">
         <v>88</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="C111" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D111" s="1"/>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="2">
+      <c r="D111" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F111" s="3"/>
+    </row>
+    <row r="112" spans="1:6" s="2" customFormat="1" ht="42.75">
+      <c r="A112" s="4"/>
+      <c r="B112" s="3">
         <v>89</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="C112" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D112" s="1"/>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="2">
+      <c r="D112" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="F112" s="3"/>
+    </row>
+    <row r="113" spans="1:6" s="2" customFormat="1" ht="71.25">
+      <c r="A113" s="4"/>
+      <c r="B113" s="3">
         <v>90</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="C113" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D113" s="1"/>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="2">
+      <c r="D113" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F113" s="3"/>
+    </row>
+    <row r="114" spans="1:6" s="2" customFormat="1" ht="28.5">
+      <c r="A114" s="4"/>
+      <c r="B114" s="15">
         <v>91</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="C114" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="D114" s="1"/>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="2">
+      <c r="D114" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="E114" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F114" s="3"/>
+    </row>
+    <row r="115" spans="1:6" s="2" customFormat="1" ht="28.5">
+      <c r="A115" s="4"/>
+      <c r="B115" s="15"/>
+      <c r="C115" s="15"/>
+      <c r="D115" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E115" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F115" s="3"/>
+    </row>
+    <row r="116" spans="1:6" s="2" customFormat="1" ht="28.5">
+      <c r="A116" s="6"/>
+      <c r="B116" s="15">
         <v>92</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="C116" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="D115" s="1"/>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="2">
+      <c r="D116" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="E116" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F116" s="3"/>
+    </row>
+    <row r="117" spans="1:6" s="2" customFormat="1" ht="28.5">
+      <c r="A117" s="6"/>
+      <c r="B117" s="15"/>
+      <c r="C117" s="15"/>
+      <c r="D117" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E117" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="F117" s="3"/>
+    </row>
+    <row r="118" spans="1:6" s="2" customFormat="1" ht="57">
+      <c r="A118" s="4"/>
+      <c r="B118" s="3">
         <v>93</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="C118" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D116" s="1"/>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="2">
+      <c r="D118" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F118" s="3"/>
+    </row>
+    <row r="119" spans="1:6" s="2" customFormat="1" ht="57">
+      <c r="A119" s="4"/>
+      <c r="B119" s="3">
         <v>94</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="C119" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D117" s="1"/>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="2">
+      <c r="D119" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E119" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F119" s="3"/>
+    </row>
+    <row r="120" spans="1:6" s="2" customFormat="1" ht="28.5">
+      <c r="A120" s="6"/>
+      <c r="B120" s="3">
         <v>95</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="C120" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D118" s="1"/>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="2">
+      <c r="D120" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="F120" s="3"/>
+    </row>
+    <row r="121" spans="1:6" s="2" customFormat="1" ht="128.25">
+      <c r="A121" s="4"/>
+      <c r="B121" s="3">
         <v>96</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="C121" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D119" s="1"/>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="2">
+      <c r="D121" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="F121" s="3"/>
+    </row>
+    <row r="122" spans="1:6" s="2" customFormat="1" ht="28.5">
+      <c r="A122" s="4"/>
+      <c r="B122" s="3">
         <v>97</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="C122" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D120" s="1"/>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="2">
+      <c r="D122" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F122" s="3"/>
+    </row>
+    <row r="123" spans="1:6" s="2" customFormat="1">
+      <c r="A123" s="4"/>
+      <c r="B123" s="15">
         <v>98</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="C123" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="D121" s="1"/>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="2">
+      <c r="D123" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F123" s="3"/>
+    </row>
+    <row r="124" spans="1:6" s="2" customFormat="1">
+      <c r="A124" s="4"/>
+      <c r="B124" s="15"/>
+      <c r="C124" s="15"/>
+      <c r="D124" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="E124" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F124" s="3"/>
+    </row>
+    <row r="125" spans="1:6" s="2" customFormat="1">
+      <c r="A125" s="4"/>
+      <c r="B125" s="15">
         <v>99</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="C125" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="D122" s="1"/>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="2">
+      <c r="D125" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="E125" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F125" s="3"/>
+    </row>
+    <row r="126" spans="1:6" s="2" customFormat="1">
+      <c r="A126" s="4"/>
+      <c r="B126" s="15"/>
+      <c r="C126" s="15"/>
+      <c r="D126" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="E126" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F126" s="3"/>
+    </row>
+    <row r="127" spans="1:6" s="2" customFormat="1" ht="57">
+      <c r="A127" s="4"/>
+      <c r="B127" s="3">
         <v>100</v>
       </c>
-      <c r="B123" s="2" t="s">
+      <c r="C127" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D123" s="1"/>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="2">
+      <c r="D127" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E127" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F127" s="3"/>
+    </row>
+    <row r="128" spans="1:6" s="2" customFormat="1" ht="28.5">
+      <c r="A128" s="4"/>
+      <c r="B128" s="3">
         <v>101</v>
       </c>
-      <c r="B124" s="2" t="s">
+      <c r="C128" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D124" s="1"/>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="2">
+      <c r="D128" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F128" s="3"/>
+    </row>
+    <row r="129" spans="1:6" s="2" customFormat="1" ht="313.5">
+      <c r="A129" s="6"/>
+      <c r="B129" s="3">
         <v>102</v>
       </c>
-      <c r="B125" s="2" t="s">
+      <c r="C129" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D125" s="1"/>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="2">
+      <c r="D129" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="E129" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="F129" s="12" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" s="2" customFormat="1" ht="85.5">
+      <c r="A130" s="6"/>
+      <c r="B130" s="3">
         <v>103</v>
       </c>
-      <c r="B126" s="2" t="s">
+      <c r="C130" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D126" s="1"/>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="2">
+      <c r="D130" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="E130" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="F130" s="3"/>
+    </row>
+    <row r="131" spans="1:6" s="2" customFormat="1" ht="71.25">
+      <c r="A131" s="6"/>
+      <c r="B131" s="3">
         <v>104</v>
       </c>
-      <c r="B127" s="2" t="s">
+      <c r="C131" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D127" s="1"/>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="2">
+      <c r="D131" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="E131" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="F131" s="3"/>
+    </row>
+    <row r="132" spans="1:6" s="2" customFormat="1">
+      <c r="A132" s="4"/>
+      <c r="B132" s="15">
         <v>105</v>
       </c>
-      <c r="B128" s="2" t="s">
+      <c r="C132" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="D128" s="1"/>
-    </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D129" s="1"/>
-    </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B130" s="1"/>
-      <c r="D130" s="1"/>
-    </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B131" s="1"/>
-      <c r="D131" s="1"/>
-    </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B132" s="1"/>
-      <c r="D132" s="1"/>
-    </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B133" s="1"/>
-      <c r="D133" s="1"/>
-    </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B134" s="1"/>
-      <c r="D134" s="1"/>
-    </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B135" s="1"/>
-      <c r="D135" s="1"/>
-    </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B136" s="1"/>
-      <c r="D136" s="1"/>
-    </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B137" s="1"/>
-      <c r="D137" s="1"/>
-    </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B138" s="1"/>
-      <c r="D138" s="1"/>
-    </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B139" s="1"/>
-      <c r="D139" s="1"/>
-    </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B140" s="1"/>
-      <c r="D140" s="1"/>
-    </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B141" s="1"/>
-      <c r="D141" s="1"/>
-    </row>
-    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B142" s="1"/>
-      <c r="D142" s="1"/>
-    </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B143" s="1"/>
-      <c r="D143" s="1"/>
-    </row>
-    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B144" s="1"/>
-      <c r="D144" s="1"/>
-    </row>
-    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B145" s="1"/>
-      <c r="D145" s="1"/>
-    </row>
-    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B146" s="1"/>
-      <c r="D146" s="1"/>
-    </row>
-    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B147" s="1"/>
-      <c r="D147" s="1"/>
-    </row>
-    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B148" s="1"/>
-      <c r="D148" s="1"/>
-    </row>
-    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B149" s="1"/>
-      <c r="D149" s="1"/>
-    </row>
-    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B150" s="1"/>
-      <c r="D150" s="1"/>
-    </row>
-    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B151" s="1"/>
-      <c r="D151" s="1"/>
-    </row>
-    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B152" s="1"/>
-      <c r="D152" s="1"/>
-    </row>
-    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B153" s="1"/>
-      <c r="D153" s="1"/>
-    </row>
-    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B154" s="1"/>
-      <c r="D154" s="1"/>
-    </row>
-    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B155" s="1"/>
-      <c r="D155" s="1"/>
-    </row>
-    <row r="156" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B156" s="1"/>
-      <c r="D156" s="1"/>
-    </row>
-    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B157" s="1"/>
-      <c r="D157" s="1"/>
-    </row>
-    <row r="158" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B158" s="1"/>
-      <c r="D158" s="1"/>
-    </row>
-    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B159" s="1"/>
-      <c r="D159" s="1"/>
-    </row>
-    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B160" s="1"/>
-      <c r="D160" s="1"/>
-    </row>
-    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B161" s="1"/>
-      <c r="D161" s="1"/>
-    </row>
-    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B162" s="1"/>
-      <c r="D162" s="1"/>
-    </row>
-    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B163" s="1"/>
-      <c r="D163" s="1"/>
+      <c r="D132" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="E132" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F132" s="3"/>
+    </row>
+    <row r="133" spans="1:6" s="2" customFormat="1" ht="409.5">
+      <c r="A133" s="6"/>
+      <c r="B133" s="15"/>
+      <c r="C133" s="15"/>
+      <c r="D133" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="E133" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="F133" s="3"/>
+    </row>
+    <row r="134" spans="1:6" s="2" customFormat="1">
+      <c r="A134" s="4"/>
+      <c r="C134" s="3"/>
+      <c r="E134" s="3"/>
+    </row>
+    <row r="135" spans="1:6" s="2" customFormat="1">
+      <c r="A135" s="4"/>
+      <c r="C135" s="3"/>
+      <c r="E135" s="3"/>
+    </row>
+    <row r="136" spans="1:6" s="2" customFormat="1">
+      <c r="A136" s="4"/>
+      <c r="C136" s="3"/>
+      <c r="E136" s="3"/>
+    </row>
+    <row r="137" spans="1:6" s="2" customFormat="1">
+      <c r="A137" s="4"/>
+      <c r="C137" s="3"/>
+      <c r="E137" s="3"/>
+    </row>
+    <row r="138" spans="1:6" s="2" customFormat="1">
+      <c r="A138" s="4"/>
+      <c r="C138" s="3"/>
+      <c r="E138" s="3"/>
+    </row>
+    <row r="139" spans="1:6" s="2" customFormat="1">
+      <c r="A139" s="4"/>
+      <c r="C139" s="3"/>
+      <c r="E139" s="3"/>
+    </row>
+    <row r="140" spans="1:6" s="2" customFormat="1">
+      <c r="A140" s="4"/>
+      <c r="C140" s="3"/>
+      <c r="E140" s="3"/>
+    </row>
+    <row r="141" spans="1:6" s="2" customFormat="1">
+      <c r="A141" s="4"/>
+      <c r="C141" s="3"/>
+      <c r="E141" s="3"/>
+    </row>
+    <row r="142" spans="1:6" s="2" customFormat="1">
+      <c r="A142" s="4"/>
+      <c r="C142" s="3"/>
+      <c r="E142" s="3"/>
+    </row>
+    <row r="143" spans="1:6" s="2" customFormat="1">
+      <c r="A143" s="4"/>
+      <c r="C143" s="3"/>
+      <c r="E143" s="3"/>
+    </row>
+    <row r="144" spans="1:6" s="2" customFormat="1">
+      <c r="A144" s="4"/>
+      <c r="C144" s="3"/>
+      <c r="E144" s="3"/>
+    </row>
+    <row r="145" spans="1:5" s="2" customFormat="1">
+      <c r="A145" s="4"/>
+      <c r="C145" s="3"/>
+      <c r="E145" s="3"/>
+    </row>
+    <row r="146" spans="1:5" s="2" customFormat="1">
+      <c r="A146" s="4"/>
+      <c r="C146" s="3"/>
+      <c r="E146" s="3"/>
+    </row>
+    <row r="147" spans="1:5" s="2" customFormat="1">
+      <c r="A147" s="4"/>
+      <c r="C147" s="3"/>
+      <c r="E147" s="3"/>
+    </row>
+    <row r="148" spans="1:5" s="2" customFormat="1">
+      <c r="A148" s="4"/>
+      <c r="C148" s="3"/>
+      <c r="E148" s="3"/>
+    </row>
+    <row r="149" spans="1:5" s="2" customFormat="1">
+      <c r="A149" s="4"/>
+      <c r="C149" s="3"/>
+      <c r="E149" s="3"/>
+    </row>
+    <row r="150" spans="1:5" s="2" customFormat="1">
+      <c r="A150" s="4"/>
+      <c r="C150" s="3"/>
+      <c r="E150" s="3"/>
+    </row>
+    <row r="151" spans="1:5" s="2" customFormat="1">
+      <c r="A151" s="4"/>
+      <c r="C151" s="3"/>
+      <c r="E151" s="3"/>
+    </row>
+    <row r="152" spans="1:5" s="2" customFormat="1">
+      <c r="A152" s="4"/>
+      <c r="C152" s="3"/>
+      <c r="E152" s="3"/>
+    </row>
+    <row r="153" spans="1:5" s="2" customFormat="1">
+      <c r="A153" s="4"/>
+      <c r="C153" s="3"/>
+      <c r="E153" s="3"/>
+    </row>
+    <row r="154" spans="1:5" s="2" customFormat="1">
+      <c r="A154" s="4"/>
+      <c r="C154" s="3"/>
+      <c r="E154" s="3"/>
+    </row>
+    <row r="155" spans="1:5" s="2" customFormat="1">
+      <c r="A155" s="4"/>
+      <c r="C155" s="3"/>
+      <c r="E155" s="3"/>
+    </row>
+    <row r="156" spans="1:5" s="2" customFormat="1">
+      <c r="A156" s="4"/>
+      <c r="C156" s="3"/>
+      <c r="E156" s="3"/>
+    </row>
+    <row r="157" spans="1:5" s="2" customFormat="1">
+      <c r="A157" s="4"/>
+      <c r="C157" s="3"/>
+      <c r="E157" s="3"/>
+    </row>
+    <row r="158" spans="1:5" s="2" customFormat="1">
+      <c r="A158" s="4"/>
+      <c r="C158" s="3"/>
+      <c r="E158" s="3"/>
+    </row>
+    <row r="159" spans="1:5" s="2" customFormat="1">
+      <c r="A159" s="4"/>
+      <c r="C159" s="3"/>
+      <c r="E159" s="3"/>
+    </row>
+    <row r="160" spans="1:5" s="2" customFormat="1">
+      <c r="A160" s="4"/>
+      <c r="C160" s="3"/>
+      <c r="E160" s="3"/>
+    </row>
+    <row r="161" spans="1:5" s="2" customFormat="1">
+      <c r="A161" s="4"/>
+      <c r="C161" s="3"/>
+      <c r="E161" s="3"/>
+    </row>
+    <row r="162" spans="1:5" s="2" customFormat="1">
+      <c r="A162" s="4"/>
+      <c r="C162" s="3"/>
+      <c r="E162" s="3"/>
+    </row>
+    <row r="163" spans="1:5" s="2" customFormat="1">
+      <c r="A163" s="4"/>
+      <c r="C163" s="3"/>
+      <c r="E163" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="22">
+    <mergeCell ref="B125:B126"/>
+    <mergeCell ref="C125:C126"/>
+    <mergeCell ref="C132:C133"/>
+    <mergeCell ref="B132:B133"/>
+    <mergeCell ref="B114:B115"/>
+    <mergeCell ref="C114:C115"/>
+    <mergeCell ref="B116:B117"/>
+    <mergeCell ref="C116:C117"/>
+    <mergeCell ref="B123:B124"/>
+    <mergeCell ref="C123:C124"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="C37:C42"/>
+    <mergeCell ref="B37:B42"/>
+    <mergeCell ref="C93:C94"/>
     <mergeCell ref="B93:B94"/>
-    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="C105:C108"/>
     <mergeCell ref="B105:B108"/>
-    <mergeCell ref="A105:A108"/>
+    <mergeCell ref="C46:C47"/>
     <mergeCell ref="B46:B47"/>
-    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="C70:C79"/>
     <mergeCell ref="B70:B79"/>
-    <mergeCell ref="A70:A79"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B37:B42"/>
-    <mergeCell ref="A37:A42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C1. Yellow - required API for Wallet
+2. Light Blue API - which provide extra features to wallet
+3. Light Orange - for API which give</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>